<commit_message>
New data for August snapshot
</commit_message>
<xml_diff>
--- a/data/monthly industry stats.xlsx
+++ b/data/monthly industry stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Documents\Rpackages\china_co2\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Documents\RPackages\china_co2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BF4955-8C2C-44BE-93AB-FCA57FA77C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBB9B42-B2E7-4BE0-B25E-3DE9F4E72445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="1520" windowWidth="27540" windowHeight="15860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Output_ Raw Coal_ YTD" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
             <sz val="9"/>
             <rFont val="宋体"/>
           </rPr>
-          <t>UEsDBBQACAgIABSk8VYAAAAAAAAAAAAAAAABAAAAMMWca28c13nH/bqfYrEvigTQIud+4TuZkmLDki2IjIMgCIrnnPMccqDZHWZ2VjJjGEiRonrlOpcCKRAEaHoNWjR1kLQwgrr9MpZlfYs+s0vKFHmWpIS9SIC0O+TO/vc3z/2c2du33nzjz954440Ph/jBUdN2u80kVwfDnQ+HCTPM6u4uTA5mcIDDnSFOhjeGqZoe1XB8r0n9oTR+e5KqCF3V9D+spjencbjTtTPsn7xVJXyzhsnDxaGPbpy8yX7V1fje0fxF9E5Q1/Mjt2sc46SbDncy1FM6Q2xmk649fvE84TS21cnrFm+SW/zhDCfx+MW7JjpFlStsT49MYXxU44tnWGPsMM3f8R08vltNu+HO94ctTrumxXdhjMPFaem/2aTqhr2O1B9M0PX/TZtZG/sHs6P+yK3+6A9eHD55mw5CvTjZqfj+XNPTH5956SmaMXZtRfC+/+HwL+iHcKs6mL9A3Fg83z8+ol/mN4YBD6rJ4qVD7p1nXPJe5CFdKXyAsWkTneUHJ7J3hnuMCeN9/zs4WUgavjfrjmbdzuABPB7sNlDvDL63f2v+C9/pPzKdmNGfQddMpsP5VYNJwvTis+AHXQux24eDs9dhuKNuDA/aZnY0/8HJ7z5EujZDBWBF8mAcBMk4yuiSjyp4K5zjPtK7TC6XdnKBXhBc6PzisydPf/rb4Uc3Xo2aZ9ek5kvUdpuHuH5iMSAoyDo67yU44xJTkTmHTMQA6SKxs7JWSotsTAh3FS3LuCrR+jZOsKUIMTkY7MIRxKo7LsEbjKu6Js8ePHx8uCKCWSWPwTnBFGiXpNbGBy5CsCzwEC4SvETqEqB/+r+nH//k2S/+5ctf/vfasCpdxArTpq4mGzDEzKzm3jJmMksmYVA6KORWG+6SUwWM56RtxRhV0XVvVUgZYPBetYGQZ21y2rLkKe7JxJEnFwPLgfhRGPQXuV0UtxVyWpbIvYNtM8VN2JtRCQx4B5acFiOTUtgchDEqKgN4kdt5adugxlnRS/dmdZ5RXh/cjFXaADryR+YMKJeiMdFz1JJhshko6Qa4iK6obyv8TLFAud0dHtcbsTpIjEG0IoKTWTlEp7MOMSvjtPCFKHde2moLFHudAsVyW/TV+zVMuypOB9VkcL+txtAeD+407Xi6fozMY9JBCG9CiikFm1NgMkmFxlIYvIjxSq1bsUZXLvwOcUzdTj24UwVsN0AzEjYGicoXSGijpOtttXQQg0whuEINWFa4DYaCFRmeXG+61k2axW4DED2KlCh1MBk1VYPZeEX/kk8bguoK+WSZxG1QlFYUKVYHg7dbYrR+fJquZGQxoaA6MEuVJGXknATYyNDrAr7z2rbDzRQ9uJ0lHOx1iPUG0KFMQvoUZc/NQgJnuRbBgw1Oh1xw34K8rdBzrFjN9MIG9+hkbQUbAegIn4s2W0whBdBRMsPRpdx/jEL8W6JwGwx1uY7ex8ngnWqSpoMmD95tJqOMLX366eAedhthGoVOgvd1dZAqWk2fJ1FK0SoH6lQK4fCairfCuFw17jZHR9hu0lBDsi7KyEFapQIBtswFJVmIAjAUxlvLJG6HYjFT36xn42oC64enFPXF5OcuoBdBK5atNJzzbAW5faFrOadsK8zKlfdC2dw5Nmd8SmqvE3C0up8XhkRPAxqPlKWDL6SZS1Rug6VlxcHh7nw5YP34nM1eRmEBDdpErpxYVtwzg5kXA+LLwrZCjJerwhqoi/o2la/LrO4xVgeH3Sg0H6wIHndIjZ40lh5pANKvRKKsHSAa70rV4UWNSwk+f/Lx8yefPPvd79fF0bFinTNPbKM46+aj4HsQD6sJDvabZtnUcLG4syKiXqBzNgYXHHcsSXJhZQ2IKKUvjQ2vVrvcRD/59BXRCsY1F1eNJoSSktkS2rcnaTbt+pAzeNCE5qJ79+K+NcVuVfMIKywZp0jZJovSZmW4icZJC4qHwirKMoFlhgTwW0//+Zfrs89iZLy5O7jXkJplXv7w8arq70x+TWKz7M9L4ZEFbb0KOfFkSvX3BWXLTW++brI2cLzY/p25uG82VV2a4eAjOGra+Yr2alvB6KTrBxFUJ3KqvANjlKqRSWO8Z5fa4TmpZaRf/fyzp5/8jMLlGtOOE8Vweb95TKXs6eIZcbv9w1l1dEnyXpl96hwTQ26VRuc5yzJlo1MGboU0UKB6tdRVG+w1J7lOlD29aklzXc/mYnebSdc29deiL5rvyZaFlYTOCNElkM6rmBWmyLNSnCcdTfSludl1xS4Npd+gUPrN9RF2ReOF+BAO+sy5GapKixykRcieekaHSjCgNI9olJelmdBlApeSXBtEWSw87yCm03HpS161VpQhhagU9dnCMJtdQsm8cdFwL7ko5farZW4BaHlOOW8xLuPYzXdcrQJj8p7LjFEnDE4E6bVFh30Z2k/dSrOLZeKW0Fvf+pdTxag5r4gHe2Osuysce3UUwQWOAoBASiGoheRMmcCD8i74Uiq6UuQKaV5ruxPRLEbIu9Ae4ODPSXCqZuPRtPoRedF+z6dp1+neWfR26Dl1PkIKio1ZUc2kMiX7bL24SPQ6Qlfl4IKxa+y8o8rE+aKDz7VujqWKnixUBOp+PKOuQvWzDm689RQuSyO2S/RtFKFWnP4W7XLT9ii0B22TtyFEStlUB7EMjMkUDfDASx6+fju8fu2ui5l7bwx1/bLEZV3lKoccxgcXMRmURkdIhoogoQBSppxuSmOjy3SucLzxCjiLbv0AqvoxHA/uNrEZN131CNdaAYEmv/Y2KW4S5RlrvRece0OFurClHY6X6FvSVv7vX68t3ZhiN3l7crB8W+PKOkcD6CBqVMbwmFSkXpxnSexiNNYX9qm8LGsbYw1uDS/XO7vVo6o+WfvcO6yOlsBLj1dmd8pQStaRGm/INkq0WWuhreMqUG9YKBmXKFzK8avPP3/+5OM1zjJ8eXvKzVlHjhGquuC4awiDwmtKxgxYsIlOH0FoargpFvp+GbHQYl+UtxzhK7uuYNwQPH+N4W4R3rv4mPwE24Pjwft4WMXNQLTEznOjc+Y+eHT9olfMOjHDXXCFIHiJzJXCZPzqSXlvib64dfRkkD8aQ8LBfehXiwnV4lFooE0bWFlMgqGk/prScr+JjyK74DFKDQwQfAHt9UVvYdnMsbLZ7tZNd1g21Rd3JYxXFjkVGPLxJAO3GpGuPlc+xKgN+GLkfFnc0vsQnv3+D2vDxotr3d+DdrJ+ExSZmyy0g8RNcJSpgSMCWG+tC6XO5aysLdw05Lgr5ui3Jx0etHSuRMmwjbNq2XB8laFRgoZ+/xkVhqC0UtJGETOV2Y4bAwX/Xa5yOcpfr2f5a17uFBu/3WZM/1No6R/U2OFp2NkA0SjBYqBiUVkGOkWODJP2DpnTvrQb8kqxW+heHC8PJe5VsW1G8VTxJXOzNWRxg6h5v1fS8RQ8RUPqsYXRwYT+Fq5CqrlK7DbAivKGgt2mbtrB/vubcHmmnaN/o7KKyvEYc46Kqsr+XktfGoqf17ZSbNeMmWLJOnfVu80kVf20Hi8Od1ZPjypHo4WhKlIgFebRONTJRoz0GEoN9RKJ27G9YrR8q5lN8bCp0+AB5rY66Fc+NzPkoTjJopfJWeoZmAx9sQOOZ6p4kindOHiF1K1ALe+0+lrpd2F6eGbfzSa4eiqHhEQeNQCnQsgryj2a6iIw1DgWQuXValfr9OJ6Tl/eo/G12Dst4o+W32ez2h4SIuM5mkj9eIjWaPL3iOgZJSZXGActV7nSzVb0R18HpSw2Nl/nxH7r9r353KCvQ8YkavGlDYM3YdrfcDB/sgz0gzuDcZNmNa6qpKcSFFXgPlEZ6o2ywIlxRgOCgkPpVrvX/BzLL8Wnf/X8H3725W9/8+rF6/VnJLy4N31vDG13dNhsJlRosh6M3tksoyJbptLKciM4c9F5sMU5+3l5K949eFXYvWeUEFwWC4LbNT6ap4Qbg9vTCPX88XzCcLfKGylTGfWcyXKRrA39NmGeeHAhMeNVsL6wCHRNyauFfGXVdQK5OHjaffDWOtcsrJbMe+OdiCIDeCOQ85CDNdax0v7WM3pWtUbxCoiKOWqvqYHqPqzr6eAb9w+brnnU1B1UcXHsm+tevQjGGTI3KYLNRirihrq/vzFxqq9KEfS6gl9nXeM1vyzkpWJ193B+P8eLW44OsR1Dvdiut5lvC2FgOEjnRn1eGikPfgQAauQSFQJZR530mebpi8/+4+mvPt/54k//+vzJJzvP/vLfn/3tf+08++N/fvW73zz98f9cNqe7/PtCXo+lEJewfOs4tc3R5kDyzJ1BCyPKPHKknOtBElIwKssgE6fOdBnILz/94xpAzjcaeMmuSNkUlxS7BOR3q36SvTmQWWdP2YWPLH2AkTIxjbx3ahTIzR0940KGZSCf/+PfrAUk1T5X1qNzkPwSkPNgtCGvdjJaDWGkY8KRisyOgIrlUc4GOISMqJcyfPpP//b87/7w1U8+X4M98mutkDNhLsH47izWCO0mTdJillSyixGjRyMVtBwFipcjjklLy2P0Z5PPOd/++89exyQJSVeN8U5L59zD+T0u/ZfGxUOMD9+Hukqnr+5v2n8v9LTV4ski8w/r/ii2jxatAb1rE6Z32ma8sGfJ+Pxrq+ggdQ9td7O7cHy/WRxydKjvBI+wrZp0cvaj7s6sru/PDw0/+uj/AVBLBwgT3gXiuQ0AAFBPAAA=</t>
+          <t>UEsDBBQACAgIAOZpD1cAAAAAAAAAAAAAAAABAAAAMMWca28c13nH/bqfYrEvigTQIud+4TuZkmLDki2IjIMgCIrnnPMccqDZHWZ2VjJjGEiRonrlOpcCKRAEaHoNWjR1kLQwgrr9MpZlfYs+s0vKFHmWpIS9SIC0O+TO/vc3z/2c2du33nzjz954440Ph/jBUdN2u80kVwfDnQ+HCTPM6u4uTA5mcIDDnSFOhjeGqZoe1XB8r0n9oTR+e5KqCF3V9D+spjencbjTtTPsn7xVJXyzhsnDxaGPbpy8yX7V1fje0fxF9E5Q1/Mjt2sc46SbDncy1FM6Q2xmk649fvE84TS21cnrFm+SW/zhDCfx+MW7JjpFlStsT49MYXxU44tnWGPsMM3f8R08vltNu+HO94ctTrumxXdhjMPFaem/2aTqhr2O1B9M0PX/TZtZG/sHs6P+yK3+6A9eHD55mw5CvTjZqfj+XNPTH5956SmaMXZtRfC+/+HwL+iHcKs6mL9A3Fg83z8+ol/mN4YBD6rJ4qVD7p1nXPJe5CFdKXyAsWkTneUHJ7J3hnuMCeN9/zs4WUgavjfrjmbdzuABPB7sNlDvDL63f2v+C9/pPzKdmNGfQddMpsP5VYNJwvTis+AHXQux24eDs9dhuKNuDA/aZnY0/8HJ7z5EujZDBWBF8mAcBMk4yuiSjyp4K5zjPtK7TC6XdnKBXhBc6PzisydPf/rb4Uc3Xo2aZ9ek5kvUdpuHuH5iMSAoyDo67yU44xJTkTmHTMQA6SKxs7JWSotsTAh3FS3LuCrR+jZOsKUIMTkY7MIRxKo7LsEbjKu6Js8ePHx8uCKCWSWPwTnBFGiXpNbGBy5CsCzwEC4SvETqEqB/+r+nH//k2S/+5ctf/vfasCpdxArTpq4mGzDEzKzm3jJmMksmYVA6KORWG+6SUwWM56RtxRhV0XVvVUgZYPBetYGQZ21y2rLkKe7JxJEnFwPLgfhRGPQXuV0UtxVyWpbIvYNtM8VN2JtRCQx4B5acFiOTUtgchDEqKgN4kdt5adugxlnRS/dmdZ5RXh/cjFXaADryR+YMKJeiMdFz1JJhshko6Qa4iK6obyv8TLFAud0dHtcbsTpIjEG0IoKTWTlEp7MOMSvjtPCFKHde2moLFHudAsVyW/TV+zVMuypOB9VkcL+txtAeD+407Xi6fozMY9JBCG9CiikFm1NgMkmFxlIYvIjxSq1bsUZXLvwOcUzdTj24UwVsN0AzEjYGicoXSGijpOtttXQQg0whuEINWFa4DYaCFRmeXG+61k2axW4DED2KlCh1MBk1VYPZeEX/kk8bguoK+WSZxG1QlFYUKVYHg7dbYrR+fJquZGQxoaA6MEuVJGXknATYyNDrAr7z2rbDzRQ9uJ0lHOx1iPUG0KFMQvoUZc/NQgJnuRbBgw1Oh1xw34K8rdBzrFjN9MIG9+hkbQUbAegIn4s2W0whBdBRMsPRpdx/jEL8W6JwGwx1uY7ex8ngnWqSpoMmD95tJqOMLX366eAedhthGoVOgvd1dZAqWk2fJ1FK0SoH6lQK4fCairfCuFw17jZHR9hu0lBDsi7KyEFapQIBtswFJVmIAjAUxlvLJG6HYjFT36xn42oC64enFPXF5OcuoBdBK5atNJzzbAW5faFrOadsK8zKlfdC2dw5Nmd8SmqvE3C0up8XhkRPAxqPlKWDL6SZS1Rug6VlxcHh7nw5YP34nM1eRmEBDdpErpxYVtwzg5kXA+LLwrZCjJerwhqoi/o2la/LrO4xVgeH3Sg0H6wIHndIjZ40lh5pANKvRKKsHSAa70rV4UWNSwk+f/Lx8yefPPvd79fF0bFinTNPbKM46+aj4HsQD6sJDvabZtnUcLG4syKiXqBzNgYXHHcsSXJhZQ2IKKUvjQ2vVrvcRD/59BXRCsY1F1eNJoSSktkS2rcnaTbt+pAzeNCE5qJ79+K+NcVuVfMIKywZp0jZJovSZmW4icZJC4qHwirKMoFlhgTwW0//+Zfrs89iZLy5O7jXkJplXv7w8arq70x+TWKz7M9L4ZEFbb0KOfFkSvX3BWXLTW++brI2cLzY/p25uG82VV2a4eAjOGra+Yr2alvB6KTrBxFUJ3KqvANjlKqRSWO8Z5fa4TmpZaRf/fyzp5/8jMLlGtOOE8Vweb95TKXs6eIZcbv9w1l1dEnyXpl96hwTQ26VRuc5yzJlo1MGboU0UKB6tdRVG+w1J7lOlD29aklzXc/mYnebSdc29deiL5rvyZaFlYTOCNElkM6rmBWmyLNSnCcdTfSludl1xS4Npd+gUPrN9RF2ReOF+BAO+sy5GapKixykRcieekaHSjCgNI9olJelmdBlApeSXBtEWSw87yCm03HpS161VpQhhagU9dnCMJtdQsm8cdFwL7ko5farZW4BaHlOOW8xLuPYzXdcrQJj8p7LjFEnDE4E6bVFh30Z2k/dSrOLZeKW0Fvf+pdTxag5r4gHe2Osuysce3UUwQWOAoBASiGoheRMmcCD8i74Uiq6UuQKaV5ruxPRLEbIu9Ae4ODPSXCqZuPRtPoRedF+z6dp1+neWfR26Dl1PkIKio1ZUc2kMiX7bL24SPQ6Qlfl4IKxa+y8o8rE+aKDz7VujqWKnixUBOp+PKOuQvWzDm689RQuSyO2S/RtFKFWnP4W7XLT9ii0B22TtyFEStlUB7EMjMkUDfDASx6+fju8fu2ui5l7bwx1/bLEZV3lKoccxgcXMRmURkdIhoogoQBSppxuSmOjy3SucLzxCjiLbv0AqvoxHA/uNrEZN131CNdaAYEmv/Y2KW4S5RlrvRece0OFurClHY6X6FvSVv7vX68t3ZhiN3l7crB8W+PKOkcD6CBqVMbwmFSkXpxnSexiNNYX9qm8LGsbYw1uDS/XO7vVo6o+WfvcO6yOlsBLj1dmd8pQStaRGm/INkq0WWuhreMqUG9YKBmXKFzK8avPP3/+5OM1zjJ8eXvKzVlHjhGquuC4awiDwmtKxgxYsIlOH0FoargpFvp+GbHQYl+UtxzhK7uuYNwQPH+N4W4R3rv4mPwE24Pjwft4WMXNQLTEznOjc+Y+eHT9olfMOjHDXXCFIHiJzJXCZPzqSXlvib64dfRkkD8aQ8LBfehXiwnV4lFooE0bWFlMgqGk/prScr+JjyK74DFKDQwQfAHt9UVvYdnMsbLZ7tZNd1g21Rd3JYxXFjkVGPLxJAO3GpGuPlc+xKgN+GLkfFnc0vsQnv3+D2vDxotr3d+DdrJ+ExSZmyy0g8RNcJSpgSMCWG+tC6XO5aysLdw05Lgr5ui3Jx0etHSuRMmwjbNq2XB8laFRgoZ+/xkVhqC0UtJGETOV2Y4bAwX/Xa5yOcpfr2f5a17uFBu/3WZM/1No6R/U2OFp2NkA0SjBYqBiUVkGOkWODJP2DpnTvrQb8kqxW+heHC8PJe5VsW1G8VTxJXOzNWRxg6h5v1fS8RQ8RUPqsYXRwYT+Fq5CqrlK7DbAivKGgt2mbtrB/vubcHmmnaN/o7KKyvEYc46Kqsr+XktfGoqf17ZSbNeMmWLJOnfVu80kVf20Hi8Od1ZPjypHo4WhKlIgFebRONTJRoz0GEoN9RKJ27G9YrR8q5lN8bCp0+AB5rY66Fc+NzPkoTjJopfJWeoZmAx9sQOOZ6p4kindOHiF1K1ALe+0+lrpd2F6eGbfzSa4eiqHhEQeNQCnQsgryj2a6iIw1DgWQuXValfr9OJ6Tl/eo/G12Dst4o+W32ez2h4SIuM5mkj9eIjWaPL3iOgZJSZXGActV7nSzVb0R18HpSw2Nl/nxH7r9r353KCvQ8YkavGlDYM3YdrfcDB/sgz0gzuDcZNmNa6qpKcSFFXgPlEZ6o2ywIlxRgOCgkPpVrvX/BzLL8Wnf/X8H3725W9/8+rF6/VnJLy4N31vDG13dNhsJlRosh6M3tksoyJbptLKciM4c9F5sMU5+3l5K949eFXYvWeUEFwWC4LbNT6ap4Qbg9vTCPX88XzCcLfKGylTGfWcyXKRrA39NmGeeHAhMeNVsL6wCHRNyauFfGXVdQK5OHjaffDWOtcsrJbMe+OdiCIDeCOQ85CDNdax0v7WM3pWtUbxCoiKOWqvqYHqPqzr6eAb9w+brnnU1B1UcXHsm+tevQjGGTI3KYLNRirihrq/vzFxqq9KEfS6gl9nXeM1vyzkpWJ193B+P8eLW44OsR1Dvdiut5lvC2FgOEjnRn1eGikPfgQAauQSFQJZR530mebpi8/+4+mvPt/54k//+vzJJzvP/vLfn/3tf+08++N/fvW73zz98f9cNqe7/PtCXo+lEJewfOs4tc3R5kDyzJ1BCyPKPHKknOtBElIwKssgE6fOdBnILz/94xpAzjcaeMmuSNkUlxS7BOR3q36SvTmQWWdP2YWPLH2AkTIxjbx3ahTIzR0940KGZSCf/+PfrAUk1T5X1qNzkPwSkPNgtCGvdjJaDWGkY8KRisyOgIrlUc4GOISMqJcyfPpP//b87/7w1U8+X4M98mutkDNhLsH47izWCO0mTdJillSyixGjRyMVtBwFipcjjklLy2P0Z5PPOd/++89exyQJSVeN8U5L59zD+T0u/ZfGxUOMD9+Hukqnr+5v2n8v9LTV4ski8w/r/ii2jxatAb1rE6Z32ma8sGfJ+Pxrq+ggdQ9td7O7cHy/WRxydKjvBI+wrZp0cvaj7s6sru/PDw0/+uj/AVBLBwgT3gXiuQ0AAFBPAAA=</t>
         </r>
       </text>
     </comment>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="161">
   <si>
     <t>Name</t>
   </si>
@@ -473,58 +473,58 @@
     <t>Time Period</t>
   </si>
   <si>
-    <t>1989-01:2023-06</t>
+    <t>1989-01:2023-07</t>
+  </si>
+  <si>
+    <t>1990-01:2023-07</t>
+  </si>
+  <si>
+    <t>1989-02:2023-07</t>
+  </si>
+  <si>
+    <t>1989-02:2023-06</t>
+  </si>
+  <si>
+    <t>1997-01:2023-06</t>
+  </si>
+  <si>
+    <t>2015-12:2023-07</t>
   </si>
   <si>
     <t>1990-01:2023-06</t>
   </si>
   <si>
-    <t>1989-02:2023-06</t>
+    <t>2009-01:2023-06</t>
   </si>
   <si>
-    <t>1989-02:2023-05</t>
+    <t>2016-02:2023-07</t>
   </si>
   <si>
-    <t>1997-01:2023-05</t>
+    <t>2001-12:2023-06</t>
   </si>
   <si>
-    <t>2015-12:2023-06</t>
+    <t>1992-01:2023-06</t>
   </si>
   <si>
-    <t>1990-01:2023-05</t>
+    <t>2000-05:2023-06</t>
   </si>
   <si>
-    <t>2009-01:2023-05</t>
-  </si>
-  <si>
-    <t>2016-02:2023-06</t>
-  </si>
-  <si>
-    <t>2001-12:2023-05</t>
-  </si>
-  <si>
-    <t>1992-01:2023-05</t>
-  </si>
-  <si>
-    <t>2000-05:2023-05</t>
-  </si>
-  <si>
-    <t>2015-02:2023-05</t>
-  </si>
-  <si>
-    <t>2010-01:2023-05</t>
+    <t>2015-02:2023-06</t>
   </si>
   <si>
     <t>2010-01:2023-06</t>
   </si>
   <si>
-    <t>2009-09:2023-06</t>
+    <t>2010-01:2023-07</t>
   </si>
   <si>
-    <t>2016-05:2023-06</t>
+    <t>2009-09:2023-07</t>
   </si>
   <si>
-    <t>2001-01:2023-06</t>
+    <t>2016-05:2023-07</t>
+  </si>
+  <si>
+    <t>2001-01:2023-07</t>
   </si>
   <si>
     <t>Source</t>
@@ -536,13 +536,10 @@
     <t>Update</t>
   </si>
   <si>
-    <t>2023-07-17</t>
+    <t>2023-08-15</t>
   </si>
   <si>
-    <t>2023-06-16</t>
-  </si>
-  <si>
-    <t>2023-06-19</t>
+    <t>2023-07-19</t>
   </si>
 </sst>
 </file>
@@ -550,10 +547,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy/mm"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm"/>
     <numFmt numFmtId="165" formatCode="#,##0.00_ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -943,19 +940,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BI414"/>
+  <dimension ref="A1:BI415"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A394" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:61">
       <c r="A1" s="1" t="str">
         <f>[1]!edb()</f>
         <v>Wind</v>
       </c>
     </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:61">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1140,7 +1137,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:61">
       <c r="A3" s="2" t="s">
         <v>61</v>
       </c>
@@ -1325,7 +1322,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:61">
       <c r="A4" s="2" t="s">
         <v>63</v>
       </c>
@@ -1510,7 +1507,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:61">
       <c r="A5" s="2" t="s">
         <v>76</v>
       </c>
@@ -1695,7 +1692,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:61">
       <c r="A6" s="2" t="s">
         <v>137</v>
       </c>
@@ -1880,7 +1877,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:61">
       <c r="A7" s="2" t="s">
         <v>156</v>
       </c>
@@ -2065,7 +2062,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:61">
       <c r="A8" s="2" t="s">
         <v>158</v>
       </c>
@@ -2145,7 +2142,7 @@
         <v>159</v>
       </c>
       <c r="AA8" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AB8" s="3" t="s">
         <v>160</v>
@@ -2160,7 +2157,7 @@
         <v>160</v>
       </c>
       <c r="AF8" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AG8" s="3" t="s">
         <v>160</v>
@@ -2250,7 +2247,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="9" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:61">
       <c r="A9" s="4">
         <v>32539</v>
       </c>
@@ -2435,7 +2432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:61">
       <c r="A10" s="4">
         <v>32567</v>
       </c>
@@ -2620,7 +2617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:61">
       <c r="A11" s="4">
         <v>32598</v>
       </c>
@@ -2805,7 +2802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:61">
       <c r="A12" s="4">
         <v>32628</v>
       </c>
@@ -2990,7 +2987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:61">
       <c r="A13" s="4">
         <v>32659</v>
       </c>
@@ -3175,7 +3172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:61">
       <c r="A14" s="4">
         <v>32689</v>
       </c>
@@ -3360,7 +3357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:61">
       <c r="A15" s="4">
         <v>32720</v>
       </c>
@@ -3545,7 +3542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:61">
       <c r="A16" s="4">
         <v>32751</v>
       </c>
@@ -3730,7 +3727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:61">
       <c r="A17" s="4">
         <v>32781</v>
       </c>
@@ -3915,7 +3912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:61">
       <c r="A18" s="4">
         <v>32812</v>
       </c>
@@ -4100,7 +4097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:61">
       <c r="A19" s="4">
         <v>32842</v>
       </c>
@@ -4285,7 +4282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:61">
       <c r="A20" s="4">
         <v>32873</v>
       </c>
@@ -4470,7 +4467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:61">
       <c r="A21" s="4">
         <v>32904</v>
       </c>
@@ -4655,7 +4652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:61">
       <c r="A22" s="4">
         <v>32932</v>
       </c>
@@ -4840,7 +4837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:61">
       <c r="A23" s="4">
         <v>32963</v>
       </c>
@@ -5025,7 +5022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:61">
       <c r="A24" s="4">
         <v>32993</v>
       </c>
@@ -5210,7 +5207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:61">
       <c r="A25" s="4">
         <v>33024</v>
       </c>
@@ -5395,7 +5392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:61">
       <c r="A26" s="4">
         <v>33054</v>
       </c>
@@ -5580,7 +5577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:61">
       <c r="A27" s="4">
         <v>33085</v>
       </c>
@@ -5765,7 +5762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:61">
       <c r="A28" s="4">
         <v>33116</v>
       </c>
@@ -5950,7 +5947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:61">
       <c r="A29" s="4">
         <v>33146</v>
       </c>
@@ -6135,7 +6132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:61">
       <c r="A30" s="4">
         <v>33177</v>
       </c>
@@ -6320,7 +6317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:61">
       <c r="A31" s="4">
         <v>33207</v>
       </c>
@@ -6505,7 +6502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:61">
       <c r="A32" s="4">
         <v>33238</v>
       </c>
@@ -6690,7 +6687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:61">
       <c r="A33" s="4">
         <v>33269</v>
       </c>
@@ -6875,7 +6872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:61">
       <c r="A34" s="4">
         <v>33297</v>
       </c>
@@ -7060,7 +7057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:61">
       <c r="A35" s="4">
         <v>33328</v>
       </c>
@@ -7245,7 +7242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:61">
       <c r="A36" s="4">
         <v>33358</v>
       </c>
@@ -7430,7 +7427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:61">
       <c r="A37" s="4">
         <v>33389</v>
       </c>
@@ -7615,7 +7612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:61">
       <c r="A38" s="4">
         <v>33419</v>
       </c>
@@ -7800,7 +7797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:61">
       <c r="A39" s="4">
         <v>33450</v>
       </c>
@@ -7985,7 +7982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:61">
       <c r="A40" s="4">
         <v>33481</v>
       </c>
@@ -8170,7 +8167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:61">
       <c r="A41" s="4">
         <v>33511</v>
       </c>
@@ -8355,7 +8352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:61">
       <c r="A42" s="4">
         <v>33542</v>
       </c>
@@ -8540,7 +8537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:61">
       <c r="A43" s="4">
         <v>33572</v>
       </c>
@@ -8725,7 +8722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:61">
       <c r="A44" s="4">
         <v>33603</v>
       </c>
@@ -8910,7 +8907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:61">
       <c r="A45" s="4">
         <v>33634</v>
       </c>
@@ -9095,7 +9092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:61">
       <c r="A46" s="4">
         <v>33663</v>
       </c>
@@ -9280,7 +9277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:61">
       <c r="A47" s="4">
         <v>33694</v>
       </c>
@@ -9465,7 +9462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:61">
       <c r="A48" s="4">
         <v>33724</v>
       </c>
@@ -9650,7 +9647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:61">
       <c r="A49" s="4">
         <v>33755</v>
       </c>
@@ -9835,7 +9832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:61">
       <c r="A50" s="4">
         <v>33785</v>
       </c>
@@ -10020,7 +10017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:61">
       <c r="A51" s="4">
         <v>33816</v>
       </c>
@@ -10205,7 +10202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:61">
       <c r="A52" s="4">
         <v>33847</v>
       </c>
@@ -10390,7 +10387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:61">
       <c r="A53" s="4">
         <v>33877</v>
       </c>
@@ -10575,7 +10572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:61">
       <c r="A54" s="4">
         <v>33908</v>
       </c>
@@ -10760,7 +10757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:61">
       <c r="A55" s="4">
         <v>33938</v>
       </c>
@@ -10945,7 +10942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:61">
       <c r="A56" s="4">
         <v>33969</v>
       </c>
@@ -11130,7 +11127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:61">
       <c r="A57" s="4">
         <v>34000</v>
       </c>
@@ -11315,7 +11312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:61">
       <c r="A58" s="4">
         <v>34028</v>
       </c>
@@ -11500,7 +11497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:61">
       <c r="A59" s="4">
         <v>34059</v>
       </c>
@@ -11685,7 +11682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:61">
       <c r="A60" s="4">
         <v>34089</v>
       </c>
@@ -11870,7 +11867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:61">
       <c r="A61" s="4">
         <v>34120</v>
       </c>
@@ -12055,7 +12052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:61">
       <c r="A62" s="4">
         <v>34150</v>
       </c>
@@ -12240,7 +12237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:61">
       <c r="A63" s="4">
         <v>34181</v>
       </c>
@@ -12425,7 +12422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:61">
       <c r="A64" s="4">
         <v>34212</v>
       </c>
@@ -12610,7 +12607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:61">
       <c r="A65" s="4">
         <v>34242</v>
       </c>
@@ -12795,7 +12792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:61">
       <c r="A66" s="4">
         <v>34273</v>
       </c>
@@ -12980,7 +12977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:61">
       <c r="A67" s="4">
         <v>34303</v>
       </c>
@@ -13165,7 +13162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:61">
       <c r="A68" s="4">
         <v>34334</v>
       </c>
@@ -13350,7 +13347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:61">
       <c r="A69" s="4">
         <v>34365</v>
       </c>
@@ -13535,7 +13532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:61">
       <c r="A70" s="4">
         <v>34393</v>
       </c>
@@ -13720,7 +13717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:61">
       <c r="A71" s="4">
         <v>34424</v>
       </c>
@@ -13905,7 +13902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:61">
       <c r="A72" s="4">
         <v>34454</v>
       </c>
@@ -14090,7 +14087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:61">
       <c r="A73" s="4">
         <v>34485</v>
       </c>
@@ -14275,7 +14272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:61">
       <c r="A74" s="4">
         <v>34515</v>
       </c>
@@ -14460,7 +14457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:61">
       <c r="A75" s="4">
         <v>34546</v>
       </c>
@@ -14645,7 +14642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:61">
       <c r="A76" s="4">
         <v>34577</v>
       </c>
@@ -14830,7 +14827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:61">
       <c r="A77" s="4">
         <v>34607</v>
       </c>
@@ -15015,7 +15012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:61">
       <c r="A78" s="4">
         <v>34638</v>
       </c>
@@ -15200,7 +15197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:61">
       <c r="A79" s="4">
         <v>34668</v>
       </c>
@@ -15385,7 +15382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:61">
       <c r="A80" s="4">
         <v>34699</v>
       </c>
@@ -15570,7 +15567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:61">
       <c r="A81" s="4">
         <v>34730</v>
       </c>
@@ -15755,7 +15752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:61">
       <c r="A82" s="4">
         <v>34758</v>
       </c>
@@ -15940,7 +15937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:61">
       <c r="A83" s="4">
         <v>34789</v>
       </c>
@@ -16125,7 +16122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:61">
       <c r="A84" s="4">
         <v>34819</v>
       </c>
@@ -16310,7 +16307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:61">
       <c r="A85" s="4">
         <v>34850</v>
       </c>
@@ -16495,7 +16492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:61">
       <c r="A86" s="4">
         <v>34880</v>
       </c>
@@ -16680,7 +16677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:61">
       <c r="A87" s="4">
         <v>34911</v>
       </c>
@@ -16865,7 +16862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:61">
       <c r="A88" s="4">
         <v>34942</v>
       </c>
@@ -17050,7 +17047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:61">
       <c r="A89" s="4">
         <v>34972</v>
       </c>
@@ -17235,7 +17232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:61">
       <c r="A90" s="4">
         <v>35003</v>
       </c>
@@ -17420,7 +17417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:61">
       <c r="A91" s="4">
         <v>35033</v>
       </c>
@@ -17605,7 +17602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:61">
       <c r="A92" s="4">
         <v>35064</v>
       </c>
@@ -17790,7 +17787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:61">
       <c r="A93" s="4">
         <v>35095</v>
       </c>
@@ -17975,7 +17972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:61">
       <c r="A94" s="4">
         <v>35124</v>
       </c>
@@ -18160,7 +18157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:61">
       <c r="A95" s="4">
         <v>35155</v>
       </c>
@@ -18345,7 +18342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:61">
       <c r="A96" s="4">
         <v>35185</v>
       </c>
@@ -18530,7 +18527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:61">
       <c r="A97" s="4">
         <v>35216</v>
       </c>
@@ -18715,7 +18712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:61">
       <c r="A98" s="4">
         <v>35246</v>
       </c>
@@ -18900,7 +18897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:61">
       <c r="A99" s="4">
         <v>35277</v>
       </c>
@@ -19085,7 +19082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:61">
       <c r="A100" s="4">
         <v>35308</v>
       </c>
@@ -19270,7 +19267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:61">
       <c r="A101" s="4">
         <v>35338</v>
       </c>
@@ -19455,7 +19452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:61">
       <c r="A102" s="4">
         <v>35369</v>
       </c>
@@ -19640,7 +19637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:61">
       <c r="A103" s="4">
         <v>35399</v>
       </c>
@@ -19825,7 +19822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:61">
       <c r="A104" s="4">
         <v>35430</v>
       </c>
@@ -20010,7 +20007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:61">
       <c r="A105" s="4">
         <v>35461</v>
       </c>
@@ -20195,7 +20192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:61">
       <c r="A106" s="4">
         <v>35489</v>
       </c>
@@ -20380,7 +20377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:61">
       <c r="A107" s="4">
         <v>35520</v>
       </c>
@@ -20565,7 +20562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:61">
       <c r="A108" s="4">
         <v>35550</v>
       </c>
@@ -20750,7 +20747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:61">
       <c r="A109" s="4">
         <v>35581</v>
       </c>
@@ -20935,7 +20932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:61">
       <c r="A110" s="4">
         <v>35611</v>
       </c>
@@ -21120,7 +21117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:61">
       <c r="A111" s="4">
         <v>35642</v>
       </c>
@@ -21305,7 +21302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:61">
       <c r="A112" s="4">
         <v>35673</v>
       </c>
@@ -21490,7 +21487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:61">
       <c r="A113" s="4">
         <v>35703</v>
       </c>
@@ -21675,7 +21672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:61">
       <c r="A114" s="4">
         <v>35734</v>
       </c>
@@ -21860,7 +21857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:61">
       <c r="A115" s="4">
         <v>35764</v>
       </c>
@@ -22045,7 +22042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:61">
       <c r="A116" s="4">
         <v>35795</v>
       </c>
@@ -22230,7 +22227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:61">
       <c r="A117" s="4">
         <v>35826</v>
       </c>
@@ -22415,7 +22412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:61">
       <c r="A118" s="4">
         <v>35854</v>
       </c>
@@ -22600,7 +22597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:61">
       <c r="A119" s="4">
         <v>35885</v>
       </c>
@@ -22785,7 +22782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:61">
       <c r="A120" s="4">
         <v>35915</v>
       </c>
@@ -22970,7 +22967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:61">
       <c r="A121" s="4">
         <v>35946</v>
       </c>
@@ -23155,7 +23152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:61">
       <c r="A122" s="4">
         <v>35976</v>
       </c>
@@ -23340,7 +23337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:61">
       <c r="A123" s="4">
         <v>36007</v>
       </c>
@@ -23525,7 +23522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:61">
       <c r="A124" s="4">
         <v>36038</v>
       </c>
@@ -23710,7 +23707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:61">
       <c r="A125" s="4">
         <v>36068</v>
       </c>
@@ -23895,7 +23892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:61">
       <c r="A126" s="4">
         <v>36099</v>
       </c>
@@ -24080,7 +24077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:61">
       <c r="A127" s="4">
         <v>36129</v>
       </c>
@@ -24265,7 +24262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:61">
       <c r="A128" s="4">
         <v>36160</v>
       </c>
@@ -24450,7 +24447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:61">
       <c r="A129" s="4">
         <v>36191</v>
       </c>
@@ -24635,7 +24632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:61">
       <c r="A130" s="4">
         <v>36219</v>
       </c>
@@ -24820,7 +24817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:61">
       <c r="A131" s="4">
         <v>36250</v>
       </c>
@@ -25005,7 +25002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:61">
       <c r="A132" s="4">
         <v>36280</v>
       </c>
@@ -25190,7 +25187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:61">
       <c r="A133" s="4">
         <v>36311</v>
       </c>
@@ -25375,7 +25372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:61">
       <c r="A134" s="4">
         <v>36341</v>
       </c>
@@ -25560,7 +25557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:61">
       <c r="A135" s="4">
         <v>36372</v>
       </c>
@@ -25745,7 +25742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:61">
       <c r="A136" s="4">
         <v>36403</v>
       </c>
@@ -25930,7 +25927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:61">
       <c r="A137" s="4">
         <v>36433</v>
       </c>
@@ -26115,7 +26112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:61">
       <c r="A138" s="4">
         <v>36464</v>
       </c>
@@ -26300,7 +26297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:61">
       <c r="A139" s="4">
         <v>36494</v>
       </c>
@@ -26485,7 +26482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:61">
       <c r="A140" s="4">
         <v>36525</v>
       </c>
@@ -26670,7 +26667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:61">
       <c r="A141" s="4">
         <v>36556</v>
       </c>
@@ -26855,7 +26852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:61">
       <c r="A142" s="4">
         <v>36585</v>
       </c>
@@ -27040,7 +27037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:61">
       <c r="A143" s="4">
         <v>36616</v>
       </c>
@@ -27225,7 +27222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:61">
       <c r="A144" s="4">
         <v>36646</v>
       </c>
@@ -27410,7 +27407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:61">
       <c r="A145" s="4">
         <v>36677</v>
       </c>
@@ -27595,7 +27592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:61">
       <c r="A146" s="4">
         <v>36707</v>
       </c>
@@ -27780,7 +27777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:61">
       <c r="A147" s="4">
         <v>36738</v>
       </c>
@@ -27965,7 +27962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:61">
       <c r="A148" s="4">
         <v>36769</v>
       </c>
@@ -28150,7 +28147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:61">
       <c r="A149" s="4">
         <v>36799</v>
       </c>
@@ -28335,7 +28332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:61">
       <c r="A150" s="4">
         <v>36830</v>
       </c>
@@ -28520,7 +28517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:61">
       <c r="A151" s="4">
         <v>36860</v>
       </c>
@@ -28705,7 +28702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:61">
       <c r="A152" s="4">
         <v>36891</v>
       </c>
@@ -28890,7 +28887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:61">
       <c r="A153" s="4">
         <v>36922</v>
       </c>
@@ -29075,7 +29072,7 @@
         <v>10.534700000000001</v>
       </c>
     </row>
-    <row r="154" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:61">
       <c r="A154" s="4">
         <v>36950</v>
       </c>
@@ -29260,7 +29257,7 @@
         <v>23.813500000000001</v>
       </c>
     </row>
-    <row r="155" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:61">
       <c r="A155" s="4">
         <v>36981</v>
       </c>
@@ -29445,7 +29442,7 @@
         <v>36.866300000000003</v>
       </c>
     </row>
-    <row r="156" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:61">
       <c r="A156" s="4">
         <v>37011</v>
       </c>
@@ -29630,7 +29627,7 @@
         <v>50.189100000000003</v>
       </c>
     </row>
-    <row r="157" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:61">
       <c r="A157" s="4">
         <v>37042</v>
       </c>
@@ -29815,7 +29812,7 @@
         <v>66.942700000000002</v>
       </c>
     </row>
-    <row r="158" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:61">
       <c r="A158" s="4">
         <v>37072</v>
       </c>
@@ -30000,7 +29997,7 @@
         <v>83.662499999999994</v>
       </c>
     </row>
-    <row r="159" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:61">
       <c r="A159" s="4">
         <v>37103</v>
       </c>
@@ -30185,7 +30182,7 @@
         <v>99.267799999999994</v>
       </c>
     </row>
-    <row r="160" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:61">
       <c r="A160" s="4">
         <v>37134</v>
       </c>
@@ -30370,7 +30367,7 @@
         <v>116.0051</v>
       </c>
     </row>
-    <row r="161" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:61">
       <c r="A161" s="4">
         <v>37164</v>
       </c>
@@ -30555,7 +30552,7 @@
         <v>132.2638</v>
       </c>
     </row>
-    <row r="162" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:61">
       <c r="A162" s="4">
         <v>37195</v>
       </c>
@@ -30740,7 +30737,7 @@
         <v>148.97470000000001</v>
       </c>
     </row>
-    <row r="163" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:61">
       <c r="A163" s="4">
         <v>37225</v>
       </c>
@@ -30925,7 +30922,7 @@
         <v>165.12020000000001</v>
       </c>
     </row>
-    <row r="164" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:61">
       <c r="A164" s="4">
         <v>37256</v>
       </c>
@@ -31110,7 +31107,7 @@
         <v>174.71889999999999</v>
       </c>
     </row>
-    <row r="165" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:61">
       <c r="A165" s="4">
         <v>37287</v>
       </c>
@@ -31295,7 +31292,7 @@
         <v>12.118</v>
       </c>
     </row>
-    <row r="166" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:61">
       <c r="A166" s="4">
         <v>37315</v>
       </c>
@@ -31480,7 +31477,7 @@
         <v>19.8139</v>
       </c>
     </row>
-    <row r="167" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:61">
       <c r="A167" s="4">
         <v>37346</v>
       </c>
@@ -31665,7 +31662,7 @@
         <v>31.792100000000001</v>
       </c>
     </row>
-    <row r="168" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:61">
       <c r="A168" s="4">
         <v>37376</v>
       </c>
@@ -31850,7 +31847,7 @@
         <v>44.706699999999998</v>
       </c>
     </row>
-    <row r="169" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:61">
       <c r="A169" s="4">
         <v>37407</v>
       </c>
@@ -32035,7 +32032,7 @@
         <v>60.9953</v>
       </c>
     </row>
-    <row r="170" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:61">
       <c r="A170" s="4">
         <v>37437</v>
       </c>
@@ -32220,7 +32217,7 @@
         <v>92.281800000000004</v>
       </c>
     </row>
-    <row r="171" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:61">
       <c r="A171" s="4">
         <v>37468</v>
       </c>
@@ -32405,7 +32402,7 @@
         <v>115.7508</v>
       </c>
     </row>
-    <row r="172" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:61">
       <c r="A172" s="4">
         <v>37499</v>
       </c>
@@ -32590,7 +32587,7 @@
         <v>143.7638</v>
       </c>
     </row>
-    <row r="173" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:61">
       <c r="A173" s="4">
         <v>37529</v>
       </c>
@@ -32775,7 +32772,7 @@
         <v>172.96</v>
       </c>
     </row>
-    <row r="174" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:61">
       <c r="A174" s="4">
         <v>37560</v>
       </c>
@@ -32960,7 +32957,7 @@
         <v>200.6936</v>
       </c>
     </row>
-    <row r="175" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:61">
       <c r="A175" s="4">
         <v>37590</v>
       </c>
@@ -33145,7 +33142,7 @@
         <v>231.04390000000001</v>
       </c>
     </row>
-    <row r="176" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:61">
       <c r="A176" s="4">
         <v>37621</v>
       </c>
@@ -33330,7 +33327,7 @@
         <v>259.05110000000002</v>
       </c>
     </row>
-    <row r="177" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:61">
       <c r="A177" s="4">
         <v>37652</v>
       </c>
@@ -33515,7 +33512,7 @@
         <v>32.492600000000003</v>
       </c>
     </row>
-    <row r="178" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:61">
       <c r="A178" s="4">
         <v>37680</v>
       </c>
@@ -33700,7 +33697,7 @@
         <v>59.534700000000001</v>
       </c>
     </row>
-    <row r="179" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:61">
       <c r="A179" s="4">
         <v>37711</v>
       </c>
@@ -33885,7 +33882,7 @@
         <v>93.298599999999993</v>
       </c>
     </row>
-    <row r="180" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:61">
       <c r="A180" s="4">
         <v>37741</v>
       </c>
@@ -34070,7 +34067,7 @@
         <v>119.2555</v>
       </c>
     </row>
-    <row r="181" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:61">
       <c r="A181" s="4">
         <v>37772</v>
       </c>
@@ -34255,7 +34252,7 @@
         <v>146.02619999999999</v>
       </c>
     </row>
-    <row r="182" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:61">
       <c r="A182" s="4">
         <v>37802</v>
       </c>
@@ -34440,7 +34437,7 @@
         <v>183.2748</v>
       </c>
     </row>
-    <row r="183" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:61">
       <c r="A183" s="4">
         <v>37833</v>
       </c>
@@ -34625,7 +34622,7 @@
         <v>227.68180000000001</v>
       </c>
     </row>
-    <row r="184" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:61">
       <c r="A184" s="4">
         <v>37864</v>
       </c>
@@ -34810,7 +34807,7 @@
         <v>265.375</v>
       </c>
     </row>
-    <row r="185" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:61">
       <c r="A185" s="4">
         <v>37894</v>
       </c>
@@ -34995,7 +34992,7 @@
         <v>308.7004</v>
       </c>
     </row>
-    <row r="186" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:61">
       <c r="A186" s="4">
         <v>37925</v>
       </c>
@@ -35180,7 +35177,7 @@
         <v>357.62</v>
       </c>
     </row>
-    <row r="187" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:61">
       <c r="A187" s="4">
         <v>37955</v>
       </c>
@@ -35365,7 +35362,7 @@
         <v>398.85329999999999</v>
       </c>
     </row>
-    <row r="188" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:61">
       <c r="A188" s="4">
         <v>37986</v>
       </c>
@@ -35550,7 +35547,7 @@
         <v>433.4205</v>
       </c>
     </row>
-    <row r="189" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:61">
       <c r="A189" s="4">
         <v>38017</v>
       </c>
@@ -35735,7 +35732,7 @@
         <v>37.790199999999999</v>
       </c>
     </row>
-    <row r="190" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:61">
       <c r="A190" s="4">
         <v>38046</v>
       </c>
@@ -35920,7 +35917,7 @@
         <v>74.725099999999998</v>
       </c>
     </row>
-    <row r="191" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:61">
       <c r="A191" s="4">
         <v>38077</v>
       </c>
@@ -36105,7 +36102,7 @@
         <v>112.17829999999999</v>
       </c>
     </row>
-    <row r="192" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:61">
       <c r="A192" s="4">
         <v>38107</v>
       </c>
@@ -36290,7 +36287,7 @@
         <v>149.1387</v>
       </c>
     </row>
-    <row r="193" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:61">
       <c r="A193" s="4">
         <v>38138</v>
       </c>
@@ -36475,7 +36472,7 @@
         <v>185.92500000000001</v>
       </c>
     </row>
-    <row r="194" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:61">
       <c r="A194" s="4">
         <v>38168</v>
       </c>
@@ -36660,7 +36657,7 @@
         <v>226.3304</v>
       </c>
     </row>
-    <row r="195" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:61">
       <c r="A195" s="4">
         <v>38199</v>
       </c>
@@ -36845,7 +36842,7 @@
         <v>270.30290000000002</v>
       </c>
     </row>
-    <row r="196" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:61">
       <c r="A196" s="4">
         <v>38230</v>
       </c>
@@ -37030,7 +37027,7 @@
         <v>320.24180000000001</v>
       </c>
     </row>
-    <row r="197" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:61">
       <c r="A197" s="4">
         <v>38260</v>
       </c>
@@ -37215,7 +37212,7 @@
         <v>369.85599999999999</v>
       </c>
     </row>
-    <row r="198" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:61">
       <c r="A198" s="4">
         <v>38291</v>
       </c>
@@ -37400,7 +37397,7 @@
         <v>421.77600000000001</v>
       </c>
     </row>
-    <row r="199" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:61">
       <c r="A199" s="4">
         <v>38321</v>
       </c>
@@ -37585,7 +37582,7 @@
         <v>461.27159999999998</v>
       </c>
     </row>
-    <row r="200" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:61">
       <c r="A200" s="4">
         <v>38352</v>
       </c>
@@ -37770,7 +37767,7 @@
         <v>500.07490000000001</v>
       </c>
     </row>
-    <row r="201" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:61">
       <c r="A201" s="4">
         <v>38383</v>
       </c>
@@ -37955,7 +37952,7 @@
         <v>47.760399999999997</v>
       </c>
     </row>
-    <row r="202" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:61">
       <c r="A202" s="4">
         <v>38411</v>
       </c>
@@ -38140,7 +38137,7 @@
         <v>88.088099999999997</v>
       </c>
     </row>
-    <row r="203" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:61">
       <c r="A203" s="4">
         <v>38442</v>
       </c>
@@ -38325,7 +38322,7 @@
         <v>129.34309999999999</v>
       </c>
     </row>
-    <row r="204" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:61">
       <c r="A204" s="4">
         <v>38472</v>
       </c>
@@ -38510,7 +38507,7 @@
         <v>170.30420000000001</v>
       </c>
     </row>
-    <row r="205" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:61">
       <c r="A205" s="4">
         <v>38503</v>
       </c>
@@ -38695,7 +38692,7 @@
         <v>215.12909999999999</v>
       </c>
     </row>
-    <row r="206" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:61">
       <c r="A206" s="4">
         <v>38533</v>
       </c>
@@ -38880,7 +38877,7 @@
         <v>259.18669999999997</v>
       </c>
     </row>
-    <row r="207" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:61">
       <c r="A207" s="4">
         <v>38564</v>
       </c>
@@ -39065,7 +39062,7 @@
         <v>307.35140000000001</v>
       </c>
     </row>
-    <row r="208" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:61">
       <c r="A208" s="4">
         <v>38595</v>
       </c>
@@ -39250,7 +39247,7 @@
         <v>357.65249999999997</v>
       </c>
     </row>
-    <row r="209" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:61">
       <c r="A209" s="4">
         <v>38625</v>
       </c>
@@ -39435,7 +39432,7 @@
         <v>405.72469999999998</v>
       </c>
     </row>
-    <row r="210" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:61">
       <c r="A210" s="4">
         <v>38656</v>
       </c>
@@ -39620,7 +39617,7 @@
         <v>448.64859999999999</v>
       </c>
     </row>
-    <row r="211" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:61">
       <c r="A211" s="4">
         <v>38686</v>
       </c>
@@ -39805,7 +39802,7 @@
         <v>487.8621</v>
       </c>
     </row>
-    <row r="212" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:61">
       <c r="A212" s="4">
         <v>38717</v>
       </c>
@@ -39990,7 +39987,7 @@
         <v>530.88239999999996</v>
       </c>
     </row>
-    <row r="213" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:61">
       <c r="A213" s="4">
         <v>38748</v>
       </c>
@@ -40175,7 +40172,7 @@
         <v>41.153799999999997</v>
       </c>
     </row>
-    <row r="214" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:61">
       <c r="A214" s="4">
         <v>38776</v>
       </c>
@@ -40360,7 +40357,7 @@
         <v>82.552099999999996</v>
       </c>
     </row>
-    <row r="215" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:61">
       <c r="A215" s="4">
         <v>38807</v>
       </c>
@@ -40545,7 +40542,7 @@
         <v>125.6622</v>
       </c>
     </row>
-    <row r="216" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:61">
       <c r="A216" s="4">
         <v>38837</v>
       </c>
@@ -40730,7 +40727,7 @@
         <v>166.5959</v>
       </c>
     </row>
-    <row r="217" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:61">
       <c r="A217" s="4">
         <v>38868</v>
       </c>
@@ -40915,7 +40912,7 @@
         <v>212.24610000000001</v>
       </c>
     </row>
-    <row r="218" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:61">
       <c r="A218" s="4">
         <v>38898</v>
       </c>
@@ -41100,7 +41097,7 @@
         <v>255.79730000000001</v>
       </c>
     </row>
-    <row r="219" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:61">
       <c r="A219" s="4">
         <v>38929</v>
       </c>
@@ -41285,7 +41282,7 @@
         <v>306.04790000000003</v>
       </c>
     </row>
-    <row r="220" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:61">
       <c r="A220" s="4">
         <v>38960</v>
       </c>
@@ -41470,7 +41467,7 @@
         <v>357.20299999999997</v>
       </c>
     </row>
-    <row r="221" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:61">
       <c r="A221" s="4">
         <v>38990</v>
       </c>
@@ -41655,7 +41652,7 @@
         <v>402.34100000000001</v>
       </c>
     </row>
-    <row r="222" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:61">
       <c r="A222" s="4">
         <v>39021</v>
       </c>
@@ -41840,7 +41837,7 @@
         <v>444.11090000000002</v>
       </c>
     </row>
-    <row r="223" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:61">
       <c r="A223" s="4">
         <v>39051</v>
       </c>
@@ -42025,7 +42022,7 @@
         <v>487.73140000000001</v>
       </c>
     </row>
-    <row r="224" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:61">
       <c r="A224" s="4">
         <v>39082</v>
       </c>
@@ -42210,7 +42207,7 @@
         <v>534.39570000000003</v>
       </c>
     </row>
-    <row r="225" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:61">
       <c r="A225" s="4">
         <v>39113</v>
       </c>
@@ -42395,7 +42392,7 @@
         <v>40.249699999999997</v>
       </c>
     </row>
-    <row r="226" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:61">
       <c r="A226" s="4">
         <v>39141</v>
       </c>
@@ -42580,7 +42577,7 @@
         <v>75.990300000000005</v>
       </c>
     </row>
-    <row r="227" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:61">
       <c r="A227" s="4">
         <v>39172</v>
       </c>
@@ -42765,7 +42762,7 @@
         <v>116.75</v>
       </c>
     </row>
-    <row r="228" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:61">
       <c r="A228" s="4">
         <v>39202</v>
       </c>
@@ -42950,7 +42947,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="229" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:61">
       <c r="A229" s="4">
         <v>39233</v>
       </c>
@@ -43135,7 +43132,7 @@
         <v>197.6</v>
       </c>
     </row>
-    <row r="230" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:61">
       <c r="A230" s="4">
         <v>39263</v>
       </c>
@@ -43320,7 +43317,7 @@
         <v>265.3</v>
       </c>
     </row>
-    <row r="231" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:61">
       <c r="A231" s="4">
         <v>39294</v>
       </c>
@@ -43505,7 +43502,7 @@
         <v>326.5</v>
       </c>
     </row>
-    <row r="232" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:61">
       <c r="A232" s="4">
         <v>39325</v>
       </c>
@@ -43690,7 +43687,7 @@
         <v>390.5</v>
       </c>
     </row>
-    <row r="233" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:61">
       <c r="A233" s="4">
         <v>39355</v>
       </c>
@@ -43875,7 +43872,7 @@
         <v>452.1</v>
       </c>
     </row>
-    <row r="234" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:61">
       <c r="A234" s="4">
         <v>39386</v>
       </c>
@@ -44060,7 +44057,7 @@
         <v>510.2</v>
       </c>
     </row>
-    <row r="235" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:61">
       <c r="A235" s="4">
         <v>39416</v>
       </c>
@@ -44245,7 +44242,7 @@
         <v>565.9</v>
       </c>
     </row>
-    <row r="236" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:61">
       <c r="A236" s="4">
         <v>39447</v>
       </c>
@@ -44430,7 +44427,7 @@
         <v>621.29999999999995</v>
       </c>
     </row>
-    <row r="237" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:61">
       <c r="A237" s="4">
         <v>39478</v>
       </c>
@@ -44615,7 +44612,7 @@
         <v>53.1</v>
       </c>
     </row>
-    <row r="238" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:61">
       <c r="A238" s="4">
         <v>39507</v>
       </c>
@@ -44800,7 +44797,7 @@
         <v>105.3</v>
       </c>
     </row>
-    <row r="239" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:61">
       <c r="A239" s="4">
         <v>39538</v>
       </c>
@@ -44985,7 +44982,7 @@
         <v>163.6</v>
       </c>
     </row>
-    <row r="240" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:61">
       <c r="A240" s="4">
         <v>39568</v>
       </c>
@@ -45170,7 +45167,7 @@
         <v>223.8</v>
       </c>
     </row>
-    <row r="241" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:61">
       <c r="A241" s="4">
         <v>39599</v>
       </c>
@@ -45355,7 +45352,7 @@
         <v>278.7</v>
       </c>
     </row>
-    <row r="242" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:61">
       <c r="A242" s="4">
         <v>39629</v>
       </c>
@@ -45540,7 +45537,7 @@
         <v>329.2</v>
       </c>
     </row>
-    <row r="243" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:61">
       <c r="A243" s="4">
         <v>39660</v>
       </c>
@@ -45725,7 +45722,7 @@
         <v>388.7</v>
       </c>
     </row>
-    <row r="244" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:61">
       <c r="A244" s="4">
         <v>39691</v>
       </c>
@@ -45910,7 +45907,7 @@
         <v>453.9</v>
       </c>
     </row>
-    <row r="245" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:61">
       <c r="A245" s="4">
         <v>39721</v>
       </c>
@@ -46095,7 +46092,7 @@
         <v>509.7</v>
       </c>
     </row>
-    <row r="246" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:61">
       <c r="A246" s="4">
         <v>39752</v>
       </c>
@@ -46280,7 +46277,7 @@
         <v>573.5</v>
       </c>
     </row>
-    <row r="247" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:61">
       <c r="A247" s="4">
         <v>39782</v>
       </c>
@@ -46465,7 +46462,7 @@
         <v>627.20000000000005</v>
       </c>
     </row>
-    <row r="248" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:61">
       <c r="A248" s="4">
         <v>39813</v>
       </c>
@@ -46650,7 +46647,7 @@
         <v>683.9</v>
       </c>
     </row>
-    <row r="249" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:61">
       <c r="A249" s="4">
         <v>39844</v>
       </c>
@@ -46835,7 +46832,7 @@
         <v>40.5</v>
       </c>
     </row>
-    <row r="250" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:61">
       <c r="A250" s="4">
         <v>39872</v>
       </c>
@@ -47020,7 +47017,7 @@
         <v>98.1</v>
       </c>
     </row>
-    <row r="251" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:61">
       <c r="A251" s="4">
         <v>39903</v>
       </c>
@@ -47205,7 +47202,7 @@
         <v>139.5</v>
       </c>
     </row>
-    <row r="252" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:61">
       <c r="A252" s="4">
         <v>39933</v>
       </c>
@@ -47390,7 +47387,7 @@
         <v>218.8</v>
       </c>
     </row>
-    <row r="253" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:61">
       <c r="A253" s="4">
         <v>39964</v>
       </c>
@@ -47575,7 +47572,7 @@
         <v>272.89999999999998</v>
       </c>
     </row>
-    <row r="254" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:61">
       <c r="A254" s="4">
         <v>39994</v>
       </c>
@@ -47760,7 +47757,7 @@
         <v>325.2</v>
       </c>
     </row>
-    <row r="255" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:61">
       <c r="A255" s="4">
         <v>40025</v>
       </c>
@@ -47945,7 +47942,7 @@
         <v>390.8</v>
       </c>
     </row>
-    <row r="256" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:61">
       <c r="A256" s="4">
         <v>40056</v>
       </c>
@@ -48130,7 +48127,7 @@
         <v>453.9</v>
       </c>
     </row>
-    <row r="257" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:61">
       <c r="A257" s="4">
         <v>40086</v>
       </c>
@@ -48315,7 +48312,7 @@
         <v>516.5</v>
       </c>
     </row>
-    <row r="258" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:61">
       <c r="A258" s="4">
         <v>40117</v>
       </c>
@@ -48500,7 +48497,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="259" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:61">
       <c r="A259" s="4">
         <v>40147</v>
       </c>
@@ -48685,7 +48682,7 @@
         <v>638.11410000000001</v>
       </c>
     </row>
-    <row r="260" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:61">
       <c r="A260" s="4">
         <v>40178</v>
       </c>
@@ -48870,7 +48867,7 @@
         <v>692.6</v>
       </c>
     </row>
-    <row r="261" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:61">
       <c r="A261" s="4">
         <v>40209</v>
       </c>
@@ -49055,7 +49052,7 @@
         <v>57.634</v>
       </c>
     </row>
-    <row r="262" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:61">
       <c r="A262" s="4">
         <v>40237</v>
       </c>
@@ -49240,7 +49237,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="263" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:61">
       <c r="A263" s="4">
         <v>40268</v>
       </c>
@@ -49425,7 +49422,7 @@
         <v>175.3</v>
       </c>
     </row>
-    <row r="264" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:61">
       <c r="A264" s="4">
         <v>40298</v>
       </c>
@@ -49610,7 +49607,7 @@
         <v>229.7</v>
       </c>
     </row>
-    <row r="265" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:61">
       <c r="A265" s="4">
         <v>40329</v>
       </c>
@@ -49795,7 +49792,7 @@
         <v>282.60000000000002</v>
       </c>
     </row>
-    <row r="266" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:61">
       <c r="A266" s="4">
         <v>40359</v>
       </c>
@@ -49980,7 +49977,7 @@
         <v>333.5</v>
       </c>
     </row>
-    <row r="267" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:61">
       <c r="A267" s="4">
         <v>40390</v>
       </c>
@@ -50165,7 +50162,7 @@
         <v>397.3</v>
       </c>
     </row>
-    <row r="268" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:61">
       <c r="A268" s="4">
         <v>40421</v>
       </c>
@@ -50350,7 +50347,7 @@
         <v>462.3</v>
       </c>
     </row>
-    <row r="269" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:61">
       <c r="A269" s="4">
         <v>40451</v>
       </c>
@@ -50535,7 +50532,7 @@
         <v>527.351</v>
       </c>
     </row>
-    <row r="270" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:61">
       <c r="A270" s="4">
         <v>40482</v>
       </c>
@@ -50720,7 +50717,7 @@
         <v>596.5</v>
       </c>
     </row>
-    <row r="271" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:61">
       <c r="A271" s="4">
         <v>40512</v>
       </c>
@@ -50905,7 +50902,7 @@
         <v>668.6</v>
       </c>
     </row>
-    <row r="272" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:61">
       <c r="A272" s="4">
         <v>40543</v>
       </c>
@@ -51090,7 +51087,7 @@
         <v>738.8</v>
       </c>
     </row>
-    <row r="273" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:61">
       <c r="A273" s="4">
         <v>40574</v>
       </c>
@@ -51275,7 +51272,7 @@
         <v>75.412499999999994</v>
       </c>
     </row>
-    <row r="274" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:61">
       <c r="A274" s="4">
         <v>40602</v>
       </c>
@@ -51460,7 +51457,7 @@
         <v>135.5</v>
       </c>
     </row>
-    <row r="275" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:61">
       <c r="A275" s="4">
         <v>40633</v>
       </c>
@@ -51645,7 +51642,7 @@
         <v>205.8</v>
       </c>
     </row>
-    <row r="276" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:61">
       <c r="A276" s="4">
         <v>40663</v>
       </c>
@@ -51830,7 +51827,7 @@
         <v>279.7</v>
       </c>
     </row>
-    <row r="277" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:61">
       <c r="A277" s="4">
         <v>40694</v>
       </c>
@@ -52015,7 +52012,7 @@
         <v>348.5</v>
       </c>
     </row>
-    <row r="278" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:61">
       <c r="A278" s="4">
         <v>40724</v>
       </c>
@@ -52200,7 +52197,7 @@
         <v>414.1</v>
       </c>
     </row>
-    <row r="279" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:61">
       <c r="A279" s="4">
         <v>40755</v>
       </c>
@@ -52385,7 +52382,7 @@
         <v>491.7</v>
       </c>
     </row>
-    <row r="280" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:61">
       <c r="A280" s="4">
         <v>40786</v>
       </c>
@@ -52570,7 +52567,7 @@
         <v>573.20000000000005</v>
       </c>
     </row>
-    <row r="281" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:61">
       <c r="A281" s="4">
         <v>40816</v>
       </c>
@@ -52755,7 +52752,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="282" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:61">
       <c r="A282" s="4">
         <v>40847</v>
       </c>
@@ -52940,7 +52937,7 @@
         <v>722.5</v>
       </c>
     </row>
-    <row r="283" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:61">
       <c r="A283" s="4">
         <v>40877</v>
       </c>
@@ -53125,7 +53122,7 @@
         <v>788.2</v>
       </c>
     </row>
-    <row r="284" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:61">
       <c r="A284" s="4">
         <v>40908</v>
       </c>
@@ -53310,7 +53307,7 @@
         <v>863.5</v>
       </c>
     </row>
-    <row r="285" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:61">
       <c r="A285" s="4">
         <v>40939</v>
       </c>
@@ -53495,7 +53492,7 @@
         <v>64.516800000000003</v>
       </c>
     </row>
-    <row r="286" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:61">
       <c r="A286" s="4">
         <v>40968</v>
       </c>
@@ -53680,7 +53677,7 @@
         <v>126.2</v>
       </c>
     </row>
-    <row r="287" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:61">
       <c r="A287" s="4">
         <v>40999</v>
       </c>
@@ -53865,7 +53862,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="288" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:61">
       <c r="A288" s="4">
         <v>41029</v>
       </c>
@@ -54050,7 +54047,7 @@
         <v>324.39999999999998</v>
       </c>
     </row>
-    <row r="289" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:61">
       <c r="A289" s="4">
         <v>41060</v>
       </c>
@@ -54235,7 +54232,7 @@
         <v>393.9</v>
       </c>
     </row>
-    <row r="290" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:61">
       <c r="A290" s="4">
         <v>41090</v>
       </c>
@@ -54420,7 +54417,7 @@
         <v>463.5</v>
       </c>
     </row>
-    <row r="291" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:61">
       <c r="A291" s="4">
         <v>41121</v>
       </c>
@@ -54605,7 +54602,7 @@
         <v>549.9</v>
       </c>
     </row>
-    <row r="292" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:61">
       <c r="A292" s="4">
         <v>41152</v>
       </c>
@@ -54790,7 +54787,7 @@
         <v>633.4</v>
       </c>
     </row>
-    <row r="293" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:61">
       <c r="A293" s="4">
         <v>41182</v>
       </c>
@@ -54975,7 +54972,7 @@
         <v>719.59479999999996</v>
       </c>
     </row>
-    <row r="294" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:61">
       <c r="A294" s="4">
         <v>41213</v>
       </c>
@@ -55160,7 +55157,7 @@
         <v>812.34109999999998</v>
       </c>
     </row>
-    <row r="295" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:61">
       <c r="A295" s="4">
         <v>41243</v>
       </c>
@@ -55345,7 +55342,7 @@
         <v>892.95349999999996</v>
       </c>
     </row>
-    <row r="296" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:61">
       <c r="A296" s="4">
         <v>41274</v>
       </c>
@@ -55530,7 +55527,7 @@
         <v>973.95010000000002</v>
       </c>
     </row>
-    <row r="297" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:61">
       <c r="A297" s="4">
         <v>41305</v>
       </c>
@@ -55715,7 +55712,7 @@
         <v>89.3</v>
       </c>
     </row>
-    <row r="298" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:61">
       <c r="A298" s="4">
         <v>41333</v>
       </c>
@@ -55900,7 +55897,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="299" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:61">
       <c r="A299" s="4">
         <v>41364</v>
       </c>
@@ -56085,7 +56082,7 @@
         <v>228.18</v>
       </c>
     </row>
-    <row r="300" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:61">
       <c r="A300" s="4">
         <v>41394</v>
       </c>
@@ -56270,7 +56267,7 @@
         <v>299.77999999999997</v>
       </c>
     </row>
-    <row r="301" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:61">
       <c r="A301" s="4">
         <v>41425</v>
       </c>
@@ -56455,7 +56452,7 @@
         <v>388.19</v>
       </c>
     </row>
-    <row r="302" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:61">
       <c r="A302" s="4">
         <v>41455</v>
       </c>
@@ -56640,7 +56637,7 @@
         <v>477.45</v>
       </c>
     </row>
-    <row r="303" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:61">
       <c r="A303" s="4">
         <v>41486</v>
       </c>
@@ -56825,7 +56822,7 @@
         <v>576.54</v>
       </c>
     </row>
-    <row r="304" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:61">
       <c r="A304" s="4">
         <v>41517</v>
       </c>
@@ -57010,7 +57007,7 @@
         <v>675.92</v>
       </c>
     </row>
-    <row r="305" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:61">
       <c r="A305" s="4">
         <v>41547</v>
       </c>
@@ -57195,7 +57192,7 @@
         <v>803.5</v>
       </c>
     </row>
-    <row r="306" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:61">
       <c r="A306" s="4">
         <v>41578</v>
       </c>
@@ -57380,7 +57377,7 @@
         <v>907.12</v>
       </c>
     </row>
-    <row r="307" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:61">
       <c r="A307" s="4">
         <v>41608</v>
       </c>
@@ -57565,7 +57562,7 @@
         <v>1002.97</v>
       </c>
     </row>
-    <row r="308" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:61">
       <c r="A308" s="4">
         <v>41639</v>
       </c>
@@ -57750,7 +57747,7 @@
         <v>1106.3399999999999</v>
       </c>
     </row>
-    <row r="309" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:61">
       <c r="A309" s="4">
         <v>41670</v>
       </c>
@@ -57935,7 +57932,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="310" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:61">
       <c r="A310" s="4">
         <v>41698</v>
       </c>
@@ -58120,7 +58117,7 @@
         <v>172.84</v>
       </c>
     </row>
-    <row r="311" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:61">
       <c r="A311" s="4">
         <v>41729</v>
       </c>
@@ -58305,7 +58302,7 @@
         <v>265.27999999999997</v>
       </c>
     </row>
-    <row r="312" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:61">
       <c r="A312" s="4">
         <v>41759</v>
       </c>
@@ -58490,7 +58487,7 @@
         <v>337.91</v>
       </c>
     </row>
-    <row r="313" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:61">
       <c r="A313" s="4">
         <v>41790</v>
       </c>
@@ -58675,7 +58672,7 @@
         <v>459.57</v>
       </c>
     </row>
-    <row r="314" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:61">
       <c r="A314" s="4">
         <v>41820</v>
       </c>
@@ -58860,7 +58857,7 @@
         <v>565.89</v>
       </c>
     </row>
-    <row r="315" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:61">
       <c r="A315" s="4">
         <v>41851</v>
       </c>
@@ -59045,7 +59042,7 @@
         <v>684.67</v>
       </c>
     </row>
-    <row r="316" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:61">
       <c r="A316" s="4">
         <v>41882</v>
       </c>
@@ -59230,7 +59227,7 @@
         <v>816.14</v>
       </c>
     </row>
-    <row r="317" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:61">
       <c r="A317" s="4">
         <v>41912</v>
       </c>
@@ -59415,7 +59412,7 @@
         <v>945.57</v>
       </c>
     </row>
-    <row r="318" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:61">
       <c r="A318" s="4">
         <v>41943</v>
       </c>
@@ -59600,7 +59597,7 @@
         <v>1065.2</v>
       </c>
     </row>
-    <row r="319" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:61">
       <c r="A319" s="4">
         <v>41973</v>
       </c>
@@ -59785,7 +59782,7 @@
         <v>1186.31</v>
       </c>
     </row>
-    <row r="320" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:61">
       <c r="A320" s="4">
         <v>42004</v>
       </c>
@@ -59970,7 +59967,7 @@
         <v>1325.38</v>
       </c>
     </row>
-    <row r="321" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:61">
       <c r="A321" s="4">
         <v>42035</v>
       </c>
@@ -60155,7 +60152,7 @@
         <v>124.31</v>
       </c>
     </row>
-    <row r="322" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:61">
       <c r="A322" s="4">
         <v>42063</v>
       </c>
@@ -60340,7 +60337,7 @@
         <v>231.39</v>
       </c>
     </row>
-    <row r="323" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:61">
       <c r="A323" s="4">
         <v>42094</v>
       </c>
@@ -60525,7 +60522,7 @@
         <v>352.79</v>
       </c>
     </row>
-    <row r="324" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:61">
       <c r="A324" s="4">
         <v>42124</v>
       </c>
@@ -60710,7 +60707,7 @@
         <v>477.1</v>
       </c>
     </row>
-    <row r="325" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:61">
       <c r="A325" s="4">
         <v>42155</v>
       </c>
@@ -60895,7 +60892,7 @@
         <v>613.9</v>
       </c>
     </row>
-    <row r="326" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:61">
       <c r="A326" s="4">
         <v>42185</v>
       </c>
@@ -61080,7 +61077,7 @@
         <v>772.1</v>
       </c>
     </row>
-    <row r="327" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:61">
       <c r="A327" s="4">
         <v>42216</v>
       </c>
@@ -61265,7 +61262,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="328" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:61">
       <c r="A328" s="4">
         <v>42247</v>
       </c>
@@ -61450,7 +61447,7 @@
         <v>1102.5999999999999</v>
       </c>
     </row>
-    <row r="329" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:61">
       <c r="A329" s="4">
         <v>42277</v>
       </c>
@@ -61635,7 +61632,7 @@
         <v>1261.5999999999999</v>
       </c>
     </row>
-    <row r="330" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:61">
       <c r="A330" s="4">
         <v>42308</v>
       </c>
@@ -61820,7 +61817,7 @@
         <v>1404.5563</v>
       </c>
     </row>
-    <row r="331" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:61">
       <c r="A331" s="4">
         <v>42338</v>
       </c>
@@ -62005,7 +62002,7 @@
         <v>1549.0897</v>
       </c>
     </row>
-    <row r="332" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:61">
       <c r="A332" s="4">
         <v>42369</v>
       </c>
@@ -62190,7 +62187,7 @@
         <v>1707.8875</v>
       </c>
     </row>
-    <row r="333" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:61">
       <c r="A333" s="4">
         <v>42429</v>
       </c>
@@ -62375,7 +62372,7 @@
         <v>284.89999999999998</v>
       </c>
     </row>
-    <row r="334" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:61">
       <c r="A334" s="4">
         <v>42460</v>
       </c>
@@ -62560,7 +62557,7 @@
         <v>470.56079999999997</v>
       </c>
     </row>
-    <row r="335" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:61">
       <c r="A335" s="4">
         <v>42490</v>
       </c>
@@ -62745,7 +62742,7 @@
         <v>620.6</v>
       </c>
     </row>
-    <row r="336" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:61">
       <c r="A336" s="4">
         <v>42521</v>
       </c>
@@ -62930,7 +62927,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="337" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:61">
       <c r="A337" s="4">
         <v>42551</v>
       </c>
@@ -63115,7 +63112,7 @@
         <v>964.5</v>
       </c>
     </row>
-    <row r="338" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:61">
       <c r="A338" s="4">
         <v>42582</v>
       </c>
@@ -63300,7 +63297,7 @@
         <v>1162.5999999999999</v>
       </c>
     </row>
-    <row r="339" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:61">
       <c r="A339" s="4">
         <v>42613</v>
       </c>
@@ -63485,7 +63482,7 @@
         <v>1364.2</v>
       </c>
     </row>
-    <row r="340" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:61">
       <c r="A340" s="4">
         <v>42643</v>
       </c>
@@ -63670,7 +63667,7 @@
         <v>1544.2</v>
       </c>
     </row>
-    <row r="341" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:61">
       <c r="A341" s="4">
         <v>42674</v>
       </c>
@@ -63855,7 +63852,7 @@
         <v>1718.8</v>
       </c>
     </row>
-    <row r="342" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:61">
       <c r="A342" s="4">
         <v>42704</v>
       </c>
@@ -64040,7 +64037,7 @@
         <v>1913.7</v>
       </c>
     </row>
-    <row r="343" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:61">
       <c r="A343" s="4">
         <v>42735</v>
       </c>
@@ -64225,7 +64222,7 @@
         <v>2127.3000000000002</v>
       </c>
     </row>
-    <row r="344" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:61">
       <c r="A344" s="4">
         <v>42794</v>
       </c>
@@ -64410,7 +64407,7 @@
         <v>333.5</v>
       </c>
     </row>
-    <row r="345" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:61">
       <c r="A345" s="4">
         <v>42825</v>
       </c>
@@ -64595,7 +64592,7 @@
         <v>547.5</v>
       </c>
     </row>
-    <row r="346" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:61">
       <c r="A346" s="4">
         <v>42855</v>
       </c>
@@ -64780,7 +64777,7 @@
         <v>750.1</v>
       </c>
     </row>
-    <row r="347" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:61">
       <c r="A347" s="4">
         <v>42886</v>
       </c>
@@ -64965,7 +64962,7 @@
         <v>954.9</v>
       </c>
     </row>
-    <row r="348" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:61">
       <c r="A348" s="4">
         <v>42916</v>
       </c>
@@ -65150,7 +65147,7 @@
         <v>1153.9000000000001</v>
       </c>
     </row>
-    <row r="349" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:61">
       <c r="A349" s="4">
         <v>42947</v>
       </c>
@@ -65335,7 +65332,7 @@
         <v>1384.7</v>
       </c>
     </row>
-    <row r="350" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:61">
       <c r="A350" s="4">
         <v>42978</v>
       </c>
@@ -65520,7 +65517,7 @@
         <v>1614.9</v>
       </c>
     </row>
-    <row r="351" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:61">
       <c r="A351" s="4">
         <v>43008</v>
       </c>
@@ -65705,7 +65702,7 @@
         <v>1834.3</v>
       </c>
     </row>
-    <row r="352" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:61">
       <c r="A352" s="4">
         <v>43039</v>
       </c>
@@ -65890,7 +65887,7 @@
         <v>2035.5</v>
       </c>
     </row>
-    <row r="353" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:61">
       <c r="A353" s="4">
         <v>43069</v>
       </c>
@@ -66075,7 +66072,7 @@
         <v>2259</v>
       </c>
     </row>
-    <row r="354" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:61">
       <c r="A354" s="4">
         <v>43100</v>
       </c>
@@ -66260,7 +66257,7 @@
         <v>2480.6999999999998</v>
       </c>
     </row>
-    <row r="355" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:61">
       <c r="A355" s="4">
         <v>43159</v>
       </c>
@@ -66445,7 +66442,7 @@
         <v>393.3</v>
       </c>
     </row>
-    <row r="356" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:61">
       <c r="A356" s="4">
         <v>43190</v>
       </c>
@@ -66630,7 +66627,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="357" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:61">
       <c r="A357" s="4">
         <v>43220</v>
       </c>
@@ -66815,7 +66812,7 @@
         <v>826.8</v>
       </c>
     </row>
-    <row r="358" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:61">
       <c r="A358" s="4">
         <v>43251</v>
       </c>
@@ -67000,7 +66997,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="359" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:61">
       <c r="A359" s="4">
         <v>43281</v>
       </c>
@@ -67185,7 +67182,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="360" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:61">
       <c r="A360" s="4">
         <v>43312</v>
       </c>
@@ -67370,7 +67367,7 @@
         <v>1564</v>
       </c>
     </row>
-    <row r="361" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:61">
       <c r="A361" s="4">
         <v>43343</v>
       </c>
@@ -67555,7 +67552,7 @@
         <v>1834.9</v>
       </c>
     </row>
-    <row r="362" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:61">
       <c r="A362" s="4">
         <v>43373</v>
       </c>
@@ -67740,7 +67737,7 @@
         <v>2088.6999999999998</v>
       </c>
     </row>
-    <row r="363" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:61">
       <c r="A363" s="4">
         <v>43404</v>
       </c>
@@ -67925,7 +67922,7 @@
         <v>2341</v>
       </c>
     </row>
-    <row r="364" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:61">
       <c r="A364" s="4">
         <v>43434</v>
       </c>
@@ -68110,7 +68107,7 @@
         <v>2638</v>
       </c>
     </row>
-    <row r="365" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:61">
       <c r="A365" s="4">
         <v>43465</v>
       </c>
@@ -68295,7 +68292,7 @@
         <v>2944</v>
       </c>
     </row>
-    <row r="366" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:61">
       <c r="A366" s="4">
         <v>43524</v>
       </c>
@@ -68480,7 +68477,7 @@
         <v>483.7</v>
       </c>
     </row>
-    <row r="367" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:61">
       <c r="A367" s="4">
         <v>43555</v>
       </c>
@@ -68665,7 +68662,7 @@
         <v>770.4</v>
       </c>
     </row>
-    <row r="368" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:61">
       <c r="A368" s="4">
         <v>43585</v>
       </c>
@@ -68850,7 +68847,7 @@
         <v>1048.4000000000001</v>
       </c>
     </row>
-    <row r="369" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:61">
       <c r="A369" s="4">
         <v>43616</v>
       </c>
@@ -69035,7 +69032,7 @@
         <v>1320.3</v>
       </c>
     </row>
-    <row r="370" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:61">
       <c r="A370" s="4">
         <v>43646</v>
       </c>
@@ -69220,7 +69217,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="371" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:61">
       <c r="A371" s="4">
         <v>43677</v>
       </c>
@@ -69405,7 +69402,7 @@
         <v>1913.2</v>
       </c>
     </row>
-    <row r="372" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:61">
       <c r="A372" s="4">
         <v>43708</v>
       </c>
@@ -69590,7 +69587,7 @@
         <v>2241.6999999999998</v>
       </c>
     </row>
-    <row r="373" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:61">
       <c r="A373" s="4">
         <v>43738</v>
       </c>
@@ -69775,7 +69772,7 @@
         <v>2538.4</v>
       </c>
     </row>
-    <row r="374" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:61">
       <c r="A374" s="4">
         <v>43769</v>
       </c>
@@ -69960,7 +69957,7 @@
         <v>2826</v>
       </c>
     </row>
-    <row r="375" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:61">
       <c r="A375" s="4">
         <v>43799</v>
       </c>
@@ -70145,7 +70142,7 @@
         <v>3151.4</v>
       </c>
     </row>
-    <row r="376" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:61">
       <c r="A376" s="4">
         <v>43830</v>
       </c>
@@ -70330,7 +70327,7 @@
         <v>3483.5</v>
       </c>
     </row>
-    <row r="377" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:61">
       <c r="A377" s="4">
         <v>43890</v>
       </c>
@@ -70515,7 +70512,7 @@
         <v>473.2</v>
       </c>
     </row>
-    <row r="378" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:61">
       <c r="A378" s="4">
         <v>43921</v>
       </c>
@@ -70700,7 +70697,7 @@
         <v>779.5</v>
       </c>
     </row>
-    <row r="379" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:61">
       <c r="A379" s="4">
         <v>43951</v>
       </c>
@@ -70885,7 +70882,7 @@
         <v>1087.2</v>
       </c>
     </row>
-    <row r="380" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:61">
       <c r="A380" s="4">
         <v>43982</v>
       </c>
@@ -71070,7 +71067,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="381" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:61">
       <c r="A381" s="4">
         <v>44012</v>
       </c>
@@ -71255,7 +71252,7 @@
         <v>1715.7</v>
       </c>
     </row>
-    <row r="382" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:61">
       <c r="A382" s="4">
         <v>44043</v>
       </c>
@@ -71440,7 +71437,7 @@
         <v>2049.8000000000002</v>
       </c>
     </row>
-    <row r="383" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:61">
       <c r="A383" s="4">
         <v>44074</v>
       </c>
@@ -71625,7 +71622,7 @@
         <v>2381.4</v>
       </c>
     </row>
-    <row r="384" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:61">
       <c r="A384" s="4">
         <v>44104</v>
       </c>
@@ -71810,7 +71807,7 @@
         <v>2700.1</v>
       </c>
     </row>
-    <row r="385" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:61">
       <c r="A385" s="4">
         <v>44135</v>
       </c>
@@ -71995,7 +71992,7 @@
         <v>2986.8</v>
       </c>
     </row>
-    <row r="386" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:61">
       <c r="A386" s="4">
         <v>44165</v>
       </c>
@@ -72180,7 +72177,7 @@
         <v>3309.7</v>
       </c>
     </row>
-    <row r="387" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:61">
       <c r="A387" s="4">
         <v>44196</v>
       </c>
@@ -72365,7 +72362,7 @@
         <v>3662.5</v>
       </c>
     </row>
-    <row r="388" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:61">
       <c r="A388" s="4">
         <v>44255</v>
       </c>
@@ -72550,7 +72547,7 @@
         <v>583.79999999999995</v>
       </c>
     </row>
-    <row r="389" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:61">
       <c r="A389" s="4">
         <v>44286</v>
       </c>
@@ -72735,7 +72732,7 @@
         <v>925.9</v>
       </c>
     </row>
-    <row r="390" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:61">
       <c r="A390" s="4">
         <v>44316</v>
       </c>
@@ -72920,7 +72917,7 @@
         <v>1249.5999999999999</v>
       </c>
     </row>
-    <row r="391" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:61">
       <c r="A391" s="4">
         <v>44347</v>
       </c>
@@ -73105,7 +73102,7 @@
         <v>1592.1</v>
       </c>
     </row>
-    <row r="392" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:61">
       <c r="A392" s="4">
         <v>44377</v>
       </c>
@@ -73290,7 +73287,7 @@
         <v>1950.9</v>
       </c>
     </row>
-    <row r="393" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:61">
       <c r="A393" s="4">
         <v>44408</v>
       </c>
@@ -73475,7 +73472,7 @@
         <v>2333</v>
       </c>
     </row>
-    <row r="394" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:61">
       <c r="A394" s="4">
         <v>44439</v>
       </c>
@@ -73660,7 +73657,7 @@
         <v>2698.5</v>
       </c>
     </row>
-    <row r="395" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:61">
       <c r="A395" s="4">
         <v>44469</v>
       </c>
@@ -73845,7 +73842,7 @@
         <v>3030.9</v>
       </c>
     </row>
-    <row r="396" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:61">
       <c r="A396" s="4">
         <v>44500</v>
       </c>
@@ -74030,7 +74027,7 @@
         <v>3366.2</v>
       </c>
     </row>
-    <row r="397" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:61">
       <c r="A397" s="4">
         <v>44530</v>
       </c>
@@ -74215,7 +74212,7 @@
         <v>3702.4</v>
       </c>
     </row>
-    <row r="398" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:61">
       <c r="A398" s="4">
         <v>44561</v>
       </c>
@@ -74400,7 +74397,7 @@
         <v>4075.2</v>
       </c>
     </row>
-    <row r="399" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:61">
       <c r="A399" s="4">
         <v>44620</v>
       </c>
@@ -74585,7 +74582,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="400" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:61">
       <c r="A400" s="4">
         <v>44651</v>
       </c>
@@ -74770,7 +74767,7 @@
         <v>989.8</v>
       </c>
     </row>
-    <row r="401" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:61">
       <c r="A401" s="4">
         <v>44681</v>
       </c>
@@ -74955,7 +74952,7 @@
         <v>1316.5</v>
       </c>
     </row>
-    <row r="402" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:61">
       <c r="A402" s="4">
         <v>44712</v>
       </c>
@@ -75140,7 +75137,7 @@
         <v>1663.3</v>
       </c>
     </row>
-    <row r="403" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:61">
       <c r="A403" s="4">
         <v>44742</v>
       </c>
@@ -75325,7 +75322,7 @@
         <v>1989.9</v>
       </c>
     </row>
-    <row r="404" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:61">
       <c r="A404" s="4">
         <v>44773</v>
       </c>
@@ -75510,7 +75507,7 @@
         <v>2359.6999999999998</v>
       </c>
     </row>
-    <row r="405" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:61">
       <c r="A405" s="4">
         <v>44804</v>
       </c>
@@ -75695,7 +75692,7 @@
         <v>2722.9</v>
       </c>
     </row>
-    <row r="406" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:61">
       <c r="A406" s="4">
         <v>44834</v>
       </c>
@@ -75880,7 +75877,7 @@
         <v>3046.4</v>
       </c>
     </row>
-    <row r="407" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:61">
       <c r="A407" s="4">
         <v>44865</v>
       </c>
@@ -76065,7 +76062,7 @@
         <v>3406.8</v>
       </c>
     </row>
-    <row r="408" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:61">
       <c r="A408" s="4">
         <v>44895</v>
       </c>
@@ -76250,7 +76247,7 @@
         <v>3780.4</v>
       </c>
     </row>
-    <row r="409" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:61">
       <c r="A409" s="4">
         <v>44926</v>
       </c>
@@ -76435,7 +76432,7 @@
         <v>4177.8</v>
       </c>
     </row>
-    <row r="410" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:61">
       <c r="A410" s="4">
         <v>44985</v>
       </c>
@@ -76620,7 +76617,7 @@
         <v>667.53959999999995</v>
       </c>
     </row>
-    <row r="411" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:61">
       <c r="A411" s="4">
         <v>45016</v>
       </c>
@@ -76805,7 +76802,7 @@
         <v>1033.2489</v>
       </c>
     </row>
-    <row r="412" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:61">
       <c r="A412" s="4">
         <v>45046</v>
       </c>
@@ -76990,7 +76987,7 @@
         <v>1378.4</v>
       </c>
     </row>
-    <row r="413" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:61">
       <c r="A413" s="4">
         <v>45077</v>
       </c>
@@ -77175,7 +77172,7 @@
         <v>1747.3</v>
       </c>
     </row>
-    <row r="414" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="414" spans="1:61">
       <c r="A414" s="4">
         <v>45107</v>
       </c>
@@ -77189,160 +77186,160 @@
         <v>41679.647199999999</v>
       </c>
       <c r="E414" s="5">
-        <v>0</v>
+        <v>7789.2</v>
       </c>
       <c r="F414" s="5">
-        <v>0</v>
+        <v>10746.4</v>
       </c>
       <c r="G414" s="5">
-        <v>0</v>
+        <v>2219</v>
       </c>
       <c r="H414" s="5">
-        <v>4684</v>
+        <v>4684.1604699999998</v>
       </c>
       <c r="I414" s="5">
-        <v>1543</v>
+        <v>1542.6132399999999</v>
       </c>
       <c r="J414" s="5">
-        <v>0</v>
+        <v>5744.4925700000003</v>
       </c>
       <c r="K414" s="5">
-        <v>3382</v>
+        <v>3381.6235799999999</v>
       </c>
       <c r="L414" s="5">
-        <v>0</v>
+        <v>3536.2606900000001</v>
       </c>
       <c r="M414" s="5">
-        <v>45156</v>
+        <v>45156.428879999999</v>
       </c>
       <c r="N414" s="5">
-        <v>53564</v>
+        <v>53564.103049999998</v>
       </c>
       <c r="O414" s="5">
-        <v>67655</v>
+        <v>67654.794800000003</v>
       </c>
       <c r="P414" s="5">
-        <v>3638</v>
+        <v>3638.2667999999999</v>
       </c>
       <c r="Q414" s="5">
-        <v>0</v>
+        <v>1081.4082000000001</v>
       </c>
       <c r="R414" s="5">
-        <v>0</v>
+        <v>4059.8476599999999</v>
       </c>
       <c r="S414" s="5">
-        <v>0</v>
+        <v>3187.5481599999998</v>
       </c>
       <c r="T414" s="5">
-        <v>95300</v>
+        <v>95300.261320000005</v>
       </c>
       <c r="U414" s="5">
-        <v>46906</v>
+        <v>46906.016380000001</v>
       </c>
       <c r="V414" s="5">
-        <v>30</v>
+        <v>29.930199999999999</v>
       </c>
       <c r="W414" s="5">
         <v>222091</v>
       </c>
       <c r="X414" s="5">
-        <v>0</v>
+        <v>18397.521110000001</v>
       </c>
       <c r="Y414" s="5">
-        <v>0</v>
+        <v>102753.8</v>
       </c>
       <c r="Z414" s="5">
-        <v>9831</v>
+        <v>9831.1024099999995</v>
       </c>
       <c r="AA414" s="5">
-        <v>0</v>
+        <v>234274</v>
       </c>
       <c r="AB414" s="5">
-        <v>0</v>
+        <v>330409</v>
       </c>
       <c r="AC414" s="5">
-        <v>0</v>
+        <v>6515</v>
       </c>
       <c r="AD414" s="5">
-        <v>0</v>
+        <v>208491.5</v>
       </c>
       <c r="AE414" s="5">
-        <v>0</v>
+        <v>430405.7</v>
       </c>
       <c r="AF414" s="5">
-        <v>0</v>
+        <v>213355</v>
       </c>
       <c r="AG414" s="5">
-        <v>0</v>
+        <v>58523</v>
       </c>
       <c r="AH414" s="5">
-        <v>0</v>
+        <v>154832</v>
       </c>
       <c r="AI414" s="5">
-        <v>0</v>
+        <v>9.1044</v>
       </c>
       <c r="AJ414" s="5">
-        <v>0</v>
+        <v>382</v>
       </c>
       <c r="AK414" s="5">
-        <v>0</v>
+        <v>112603.76658</v>
       </c>
       <c r="AL414" s="5">
-        <v>0</v>
+        <v>1571.83374</v>
       </c>
       <c r="AM414" s="5">
-        <v>1310.3</v>
+        <v>1310.3394000000001</v>
       </c>
       <c r="AN414" s="5">
         <v>361.1</v>
       </c>
       <c r="AO414" s="5">
-        <v>0</v>
+        <v>6755.53442</v>
       </c>
       <c r="AP414" s="5">
-        <v>152</v>
+        <v>151.92487</v>
       </c>
       <c r="AQ414" s="5">
-        <v>0</v>
+        <v>1103.1062999999999</v>
       </c>
       <c r="AR414" s="5">
-        <v>16570000</v>
+        <v>16572627.1</v>
       </c>
       <c r="AS414" s="5">
-        <v>0</v>
+        <v>16934.6152</v>
       </c>
       <c r="AT414" s="5">
-        <v>16249</v>
+        <v>16248.5594</v>
       </c>
       <c r="AU414" s="5">
-        <v>0</v>
+        <v>9317.6731</v>
       </c>
       <c r="AV414" s="5">
-        <v>0</v>
+        <v>14059.9076</v>
       </c>
       <c r="AW414" s="5">
-        <v>0</v>
+        <v>4738.6547</v>
       </c>
       <c r="AX414" s="5">
-        <v>0</v>
+        <v>4913.0065999999997</v>
       </c>
       <c r="AY414" s="5">
-        <v>0</v>
+        <v>1202.1164000000001</v>
       </c>
       <c r="AZ414" s="5">
-        <v>0</v>
+        <v>345.2251</v>
       </c>
       <c r="BA414" s="5">
         <v>50747</v>
       </c>
       <c r="BB414" s="5">
-        <v>0</v>
+        <v>74.5</v>
       </c>
       <c r="BC414" s="5">
-        <v>0</v>
+        <v>601</v>
       </c>
       <c r="BD414" s="5">
-        <v>23241</v>
+        <v>23241.1</v>
       </c>
       <c r="BE414" s="5">
         <v>29456.973000000002</v>
@@ -77358,6 +77355,191 @@
       </c>
       <c r="BI414" s="5">
         <v>2118.8629000000001</v>
+      </c>
+    </row>
+    <row r="415" spans="1:61">
+      <c r="A415" s="4">
+        <v>45138</v>
+      </c>
+      <c r="B415" s="5">
+        <v>267182</v>
+      </c>
+      <c r="C415" s="5">
+        <v>28434</v>
+      </c>
+      <c r="D415" s="5">
+        <v>50130</v>
+      </c>
+      <c r="E415" s="5">
+        <v>0</v>
+      </c>
+      <c r="F415" s="5">
+        <v>0</v>
+      </c>
+      <c r="G415" s="5">
+        <v>0</v>
+      </c>
+      <c r="H415" s="5">
+        <v>5443</v>
+      </c>
+      <c r="I415" s="5">
+        <v>1783</v>
+      </c>
+      <c r="J415" s="5">
+        <v>0</v>
+      </c>
+      <c r="K415" s="5">
+        <v>3988</v>
+      </c>
+      <c r="L415" s="5">
+        <v>0</v>
+      </c>
+      <c r="M415" s="5">
+        <v>52892</v>
+      </c>
+      <c r="N415" s="5">
+        <v>62651</v>
+      </c>
+      <c r="O415" s="5">
+        <v>78900</v>
+      </c>
+      <c r="P415" s="5">
+        <v>4232</v>
+      </c>
+      <c r="Q415" s="5">
+        <v>0</v>
+      </c>
+      <c r="R415" s="5">
+        <v>0</v>
+      </c>
+      <c r="S415" s="5">
+        <v>0</v>
+      </c>
+      <c r="T415" s="5">
+        <v>112677</v>
+      </c>
+      <c r="U415" s="5">
+        <v>55054</v>
+      </c>
+      <c r="V415" s="5">
+        <v>35</v>
+      </c>
+      <c r="W415" s="5">
+        <v>256260</v>
+      </c>
+      <c r="X415" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y415" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z415" s="5">
+        <v>10958</v>
+      </c>
+      <c r="AA415" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB415" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC415" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD415" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE415" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF415" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG415" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH415" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI415" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ415" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK415" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL415" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM415" s="5">
+        <v>1540.8</v>
+      </c>
+      <c r="AN415" s="5">
+        <v>435.8</v>
+      </c>
+      <c r="AO415" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP415" s="5">
+        <v>176</v>
+      </c>
+      <c r="AQ415" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR415" s="5">
+        <v>19120000</v>
+      </c>
+      <c r="AS415" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT415" s="5">
+        <v>18877</v>
+      </c>
+      <c r="AU415" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV415" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW415" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX415" s="5">
+        <v>0</v>
+      </c>
+      <c r="AY415" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ415" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA415" s="5">
+        <v>59251</v>
+      </c>
+      <c r="BB415" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC415" s="5">
+        <v>0</v>
+      </c>
+      <c r="BD415" s="5">
+        <v>27661</v>
+      </c>
+      <c r="BE415" s="5">
+        <v>35474</v>
+      </c>
+      <c r="BF415" s="5">
+        <v>5717</v>
+      </c>
+      <c r="BG415" s="5">
+        <v>4836</v>
+      </c>
+      <c r="BH415" s="5">
+        <v>1604</v>
+      </c>
+      <c r="BI415" s="5">
+        <v>2499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>